<commit_message>
Converted code into a virtual computed property, renamed Id to BaseValueId, and added a new Id property.
</commit_message>
<xml_diff>
--- a/Utilities/Database/TestData/Integration.xlsx
+++ b/Utilities/Database/TestData/Integration.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Archvega\WoodseatsScouts\Utilities\Database\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B2AB43-68F7-47F5-890D-9BFF845EBA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739E270B-BBE4-41FB-9747-AD8EF42B532C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{C93039CC-B653-44F1-B956-88998CCCD8C6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{C93039CC-B653-44F1-B956-88998CCCD8C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Troops" sheetId="3" r:id="rId1"/>
     <sheet name="Sections" sheetId="4" r:id="rId2"/>
-    <sheet name="Members" sheetId="1" r:id="rId3"/>
+    <sheet name="Coins" sheetId="5" r:id="rId3"/>
+    <sheet name="Members" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Members!$A$1:$K$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Members!$A$1:$K$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="186">
   <si>
     <t>Id</t>
   </si>
@@ -171,6 +172,432 @@
   </si>
   <si>
     <t>Scouts</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>C0001099003</t>
+  </si>
+  <si>
+    <t>C0002099003</t>
+  </si>
+  <si>
+    <t>C0003099003</t>
+  </si>
+  <si>
+    <t>C0004099003</t>
+  </si>
+  <si>
+    <t>C0005099003</t>
+  </si>
+  <si>
+    <t>C0006099003</t>
+  </si>
+  <si>
+    <t>C0007099003</t>
+  </si>
+  <si>
+    <t>C0008099003</t>
+  </si>
+  <si>
+    <t>C0009099003</t>
+  </si>
+  <si>
+    <t>C0010099003</t>
+  </si>
+  <si>
+    <t>C0011099003</t>
+  </si>
+  <si>
+    <t>C0012099003</t>
+  </si>
+  <si>
+    <t>C0013099003</t>
+  </si>
+  <si>
+    <t>C0014099003</t>
+  </si>
+  <si>
+    <t>C0015099003</t>
+  </si>
+  <si>
+    <t>C0016099003</t>
+  </si>
+  <si>
+    <t>C0017099003</t>
+  </si>
+  <si>
+    <t>C0018099003</t>
+  </si>
+  <si>
+    <t>C0019099003</t>
+  </si>
+  <si>
+    <t>C0020099003</t>
+  </si>
+  <si>
+    <t>C0021099003</t>
+  </si>
+  <si>
+    <t>C0022099003</t>
+  </si>
+  <si>
+    <t>C0023099003</t>
+  </si>
+  <si>
+    <t>C0024099003</t>
+  </si>
+  <si>
+    <t>C0025099003</t>
+  </si>
+  <si>
+    <t>C0026099003</t>
+  </si>
+  <si>
+    <t>C0027099003</t>
+  </si>
+  <si>
+    <t>C0028099003</t>
+  </si>
+  <si>
+    <t>C0029099003</t>
+  </si>
+  <si>
+    <t>C0030099003</t>
+  </si>
+  <si>
+    <t>C0031099003</t>
+  </si>
+  <si>
+    <t>C0032099003</t>
+  </si>
+  <si>
+    <t>C0033099003</t>
+  </si>
+  <si>
+    <t>C0034099003</t>
+  </si>
+  <si>
+    <t>C0035099003</t>
+  </si>
+  <si>
+    <t>C0036099003</t>
+  </si>
+  <si>
+    <t>C0037099003</t>
+  </si>
+  <si>
+    <t>C0038099003</t>
+  </si>
+  <si>
+    <t>C0039099003</t>
+  </si>
+  <si>
+    <t>C0040099003</t>
+  </si>
+  <si>
+    <t>C0041099003</t>
+  </si>
+  <si>
+    <t>C0042099003</t>
+  </si>
+  <si>
+    <t>C0043099003</t>
+  </si>
+  <si>
+    <t>C0044099003</t>
+  </si>
+  <si>
+    <t>C0045099003</t>
+  </si>
+  <si>
+    <t>C0046099003</t>
+  </si>
+  <si>
+    <t>C0047099003</t>
+  </si>
+  <si>
+    <t>C0048099003</t>
+  </si>
+  <si>
+    <t>C0049099003</t>
+  </si>
+  <si>
+    <t>C0050099003</t>
+  </si>
+  <si>
+    <t>C0051099003</t>
+  </si>
+  <si>
+    <t>C0052099003</t>
+  </si>
+  <si>
+    <t>C0053099003</t>
+  </si>
+  <si>
+    <t>C0054099003</t>
+  </si>
+  <si>
+    <t>C0055099003</t>
+  </si>
+  <si>
+    <t>C0056099003</t>
+  </si>
+  <si>
+    <t>C0057099003</t>
+  </si>
+  <si>
+    <t>C0058099003</t>
+  </si>
+  <si>
+    <t>C0059099003</t>
+  </si>
+  <si>
+    <t>C0060099003</t>
+  </si>
+  <si>
+    <t>C0061099003</t>
+  </si>
+  <si>
+    <t>C0062099003</t>
+  </si>
+  <si>
+    <t>C0063099003</t>
+  </si>
+  <si>
+    <t>C0064099003</t>
+  </si>
+  <si>
+    <t>C0065099003</t>
+  </si>
+  <si>
+    <t>C0066099003</t>
+  </si>
+  <si>
+    <t>C0067099003</t>
+  </si>
+  <si>
+    <t>C0068099003</t>
+  </si>
+  <si>
+    <t>C0069099003</t>
+  </si>
+  <si>
+    <t>C0070099003</t>
+  </si>
+  <si>
+    <t>C0071099003</t>
+  </si>
+  <si>
+    <t>C0072099003</t>
+  </si>
+  <si>
+    <t>C0073099003</t>
+  </si>
+  <si>
+    <t>C0074099003</t>
+  </si>
+  <si>
+    <t>C0075099003</t>
+  </si>
+  <si>
+    <t>C0076099003</t>
+  </si>
+  <si>
+    <t>C0077099003</t>
+  </si>
+  <si>
+    <t>C0078099003</t>
+  </si>
+  <si>
+    <t>C0079099003</t>
+  </si>
+  <si>
+    <t>C0080099003</t>
+  </si>
+  <si>
+    <t>C0081001010</t>
+  </si>
+  <si>
+    <t>C0082001010</t>
+  </si>
+  <si>
+    <t>C0083001010</t>
+  </si>
+  <si>
+    <t>C0084001010</t>
+  </si>
+  <si>
+    <t>C0085001010</t>
+  </si>
+  <si>
+    <t>C0086001010</t>
+  </si>
+  <si>
+    <t>C0087001010</t>
+  </si>
+  <si>
+    <t>C0088001010</t>
+  </si>
+  <si>
+    <t>C0089001010</t>
+  </si>
+  <si>
+    <t>C0090001010</t>
+  </si>
+  <si>
+    <t>C0091001010</t>
+  </si>
+  <si>
+    <t>C0092001010</t>
+  </si>
+  <si>
+    <t>C0093001010</t>
+  </si>
+  <si>
+    <t>C0094001010</t>
+  </si>
+  <si>
+    <t>C0095001010</t>
+  </si>
+  <si>
+    <t>C0096001010</t>
+  </si>
+  <si>
+    <t>C0097001010</t>
+  </si>
+  <si>
+    <t>C0098001010</t>
+  </si>
+  <si>
+    <t>C0099001010</t>
+  </si>
+  <si>
+    <t>C0100001010</t>
+  </si>
+  <si>
+    <t>C0101001010</t>
+  </si>
+  <si>
+    <t>C0102001010</t>
+  </si>
+  <si>
+    <t>C0103001010</t>
+  </si>
+  <si>
+    <t>C0104001010</t>
+  </si>
+  <si>
+    <t>C0105001010</t>
+  </si>
+  <si>
+    <t>C0106001010</t>
+  </si>
+  <si>
+    <t>C0107001010</t>
+  </si>
+  <si>
+    <t>C0108001010</t>
+  </si>
+  <si>
+    <t>C0109001010</t>
+  </si>
+  <si>
+    <t>C0110001010</t>
+  </si>
+  <si>
+    <t>C0111001010</t>
+  </si>
+  <si>
+    <t>C0112001010</t>
+  </si>
+  <si>
+    <t>C0113001010</t>
+  </si>
+  <si>
+    <t>C0114001010</t>
+  </si>
+  <si>
+    <t>C0115001010</t>
+  </si>
+  <si>
+    <t>C0116001010</t>
+  </si>
+  <si>
+    <t>C0117001010</t>
+  </si>
+  <si>
+    <t>C0118001010</t>
+  </si>
+  <si>
+    <t>C0119001010</t>
+  </si>
+  <si>
+    <t>C0120001010</t>
+  </si>
+  <si>
+    <t>C0121001010</t>
+  </si>
+  <si>
+    <t>C0122001010</t>
+  </si>
+  <si>
+    <t>C0123001010</t>
+  </si>
+  <si>
+    <t>C0124001010</t>
+  </si>
+  <si>
+    <t>C0125001010</t>
+  </si>
+  <si>
+    <t>C0126001010</t>
+  </si>
+  <si>
+    <t>C0127001010</t>
+  </si>
+  <si>
+    <t>C0128001010</t>
+  </si>
+  <si>
+    <t>C0129001010</t>
+  </si>
+  <si>
+    <t>C0130001010</t>
+  </si>
+  <si>
+    <t>C0131001010</t>
+  </si>
+  <si>
+    <t>C0132001010</t>
+  </si>
+  <si>
+    <t>C0133001010</t>
+  </si>
+  <si>
+    <t>C0134001010</t>
+  </si>
+  <si>
+    <t>C0135001010</t>
+  </si>
+  <si>
+    <t>C0136001010</t>
+  </si>
+  <si>
+    <t>C0137001010</t>
+  </si>
+  <si>
+    <t>C0138001010</t>
+  </si>
+  <si>
+    <t>C0139001010</t>
+  </si>
+  <si>
+    <t>C0140001010</t>
   </si>
 </sst>
 </file>
@@ -581,7 +1008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56AAAD7-6ED1-44AF-A3DA-F5C94A437EA3}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -639,6 +1066,2002 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF5B841-6C68-4ACF-98A3-EA63C86CF067}">
+  <dimension ref="A1:D141"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>99</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>99</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>99</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>99</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>99</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>99</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>99</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>99</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>99</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>99</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>99</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>99</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>99</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>99</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>99</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>99</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>99</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>99</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>99</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>99</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>99</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>99</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>99</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>99</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>99</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>99</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>99</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>99</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>99</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>99</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>99</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>99</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>99</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>99</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>99</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>99</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>99</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>99</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>99</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>99</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>99</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>99</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>99</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>99</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>99</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>99</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>99</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+      <c r="D48" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>99</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>99</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>99</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+      <c r="D51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>99</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>99</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>99</v>
+      </c>
+      <c r="C54">
+        <v>3</v>
+      </c>
+      <c r="D54" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>99</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>99</v>
+      </c>
+      <c r="C56">
+        <v>3</v>
+      </c>
+      <c r="D56" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>99</v>
+      </c>
+      <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="D57" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>99</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
+      </c>
+      <c r="D58" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>99</v>
+      </c>
+      <c r="C59">
+        <v>3</v>
+      </c>
+      <c r="D59" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>99</v>
+      </c>
+      <c r="C60">
+        <v>3</v>
+      </c>
+      <c r="D60" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>99</v>
+      </c>
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>99</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>99</v>
+      </c>
+      <c r="C63">
+        <v>3</v>
+      </c>
+      <c r="D63" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>99</v>
+      </c>
+      <c r="C64">
+        <v>3</v>
+      </c>
+      <c r="D64" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>99</v>
+      </c>
+      <c r="C65">
+        <v>3</v>
+      </c>
+      <c r="D65" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>99</v>
+      </c>
+      <c r="C66">
+        <v>3</v>
+      </c>
+      <c r="D66" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>99</v>
+      </c>
+      <c r="C67">
+        <v>3</v>
+      </c>
+      <c r="D67" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>99</v>
+      </c>
+      <c r="C68">
+        <v>3</v>
+      </c>
+      <c r="D68" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>99</v>
+      </c>
+      <c r="C69">
+        <v>3</v>
+      </c>
+      <c r="D69" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>99</v>
+      </c>
+      <c r="C70">
+        <v>3</v>
+      </c>
+      <c r="D70" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>99</v>
+      </c>
+      <c r="C71">
+        <v>3</v>
+      </c>
+      <c r="D71" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>99</v>
+      </c>
+      <c r="C72">
+        <v>3</v>
+      </c>
+      <c r="D72" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>99</v>
+      </c>
+      <c r="C73">
+        <v>3</v>
+      </c>
+      <c r="D73" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>99</v>
+      </c>
+      <c r="C74">
+        <v>3</v>
+      </c>
+      <c r="D74" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>99</v>
+      </c>
+      <c r="C75">
+        <v>3</v>
+      </c>
+      <c r="D75" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>99</v>
+      </c>
+      <c r="C76">
+        <v>3</v>
+      </c>
+      <c r="D76" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>99</v>
+      </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>99</v>
+      </c>
+      <c r="C78">
+        <v>3</v>
+      </c>
+      <c r="D78" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>99</v>
+      </c>
+      <c r="C79">
+        <v>3</v>
+      </c>
+      <c r="D79" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>99</v>
+      </c>
+      <c r="C80">
+        <v>3</v>
+      </c>
+      <c r="D80" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>99</v>
+      </c>
+      <c r="C81">
+        <v>3</v>
+      </c>
+      <c r="D81" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82">
+        <v>10</v>
+      </c>
+      <c r="D82" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="C83">
+        <v>10</v>
+      </c>
+      <c r="D83" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84">
+        <v>10</v>
+      </c>
+      <c r="D84" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="C85">
+        <v>10</v>
+      </c>
+      <c r="D85" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="C86">
+        <v>10</v>
+      </c>
+      <c r="D86" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="C87">
+        <v>10</v>
+      </c>
+      <c r="D87" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>1</v>
+      </c>
+      <c r="C88">
+        <v>10</v>
+      </c>
+      <c r="D88" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>1</v>
+      </c>
+      <c r="C89">
+        <v>10</v>
+      </c>
+      <c r="D89" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>1</v>
+      </c>
+      <c r="C90">
+        <v>10</v>
+      </c>
+      <c r="D90" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91">
+        <v>10</v>
+      </c>
+      <c r="D91" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="C92">
+        <v>10</v>
+      </c>
+      <c r="D92" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <v>1</v>
+      </c>
+      <c r="C93">
+        <v>10</v>
+      </c>
+      <c r="D93" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
+      <c r="C94">
+        <v>10</v>
+      </c>
+      <c r="D94" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="C95">
+        <v>10</v>
+      </c>
+      <c r="D95" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="C96">
+        <v>10</v>
+      </c>
+      <c r="D96" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+      <c r="C97">
+        <v>10</v>
+      </c>
+      <c r="D97" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <v>1</v>
+      </c>
+      <c r="C98">
+        <v>10</v>
+      </c>
+      <c r="D98" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <v>1</v>
+      </c>
+      <c r="C99">
+        <v>10</v>
+      </c>
+      <c r="D99" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <v>1</v>
+      </c>
+      <c r="C100">
+        <v>10</v>
+      </c>
+      <c r="D100" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
+      <c r="C101">
+        <v>10</v>
+      </c>
+      <c r="D101" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102">
+        <v>10</v>
+      </c>
+      <c r="D102" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103">
+        <v>1</v>
+      </c>
+      <c r="C103">
+        <v>10</v>
+      </c>
+      <c r="D103" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104">
+        <v>10</v>
+      </c>
+      <c r="D104" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105">
+        <v>1</v>
+      </c>
+      <c r="C105">
+        <v>10</v>
+      </c>
+      <c r="D105" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106">
+        <v>1</v>
+      </c>
+      <c r="C106">
+        <v>10</v>
+      </c>
+      <c r="D106" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
+      <c r="C107">
+        <v>10</v>
+      </c>
+      <c r="D107" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108">
+        <v>1</v>
+      </c>
+      <c r="C108">
+        <v>10</v>
+      </c>
+      <c r="D108" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109">
+        <v>1</v>
+      </c>
+      <c r="C109">
+        <v>10</v>
+      </c>
+      <c r="D109" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110">
+        <v>1</v>
+      </c>
+      <c r="C110">
+        <v>10</v>
+      </c>
+      <c r="D110" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+      <c r="C111">
+        <v>10</v>
+      </c>
+      <c r="D111" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112">
+        <v>1</v>
+      </c>
+      <c r="C112">
+        <v>10</v>
+      </c>
+      <c r="D112" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113">
+        <v>1</v>
+      </c>
+      <c r="C113">
+        <v>10</v>
+      </c>
+      <c r="D113" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114">
+        <v>1</v>
+      </c>
+      <c r="C114">
+        <v>10</v>
+      </c>
+      <c r="D114" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115">
+        <v>1</v>
+      </c>
+      <c r="C115">
+        <v>10</v>
+      </c>
+      <c r="D115" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116">
+        <v>1</v>
+      </c>
+      <c r="C116">
+        <v>10</v>
+      </c>
+      <c r="D116" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117">
+        <v>1</v>
+      </c>
+      <c r="C117">
+        <v>10</v>
+      </c>
+      <c r="D117" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118">
+        <v>1</v>
+      </c>
+      <c r="C118">
+        <v>10</v>
+      </c>
+      <c r="D118" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119">
+        <v>1</v>
+      </c>
+      <c r="C119">
+        <v>10</v>
+      </c>
+      <c r="D119" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120">
+        <v>1</v>
+      </c>
+      <c r="C120">
+        <v>10</v>
+      </c>
+      <c r="D120" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121">
+        <v>1</v>
+      </c>
+      <c r="C121">
+        <v>10</v>
+      </c>
+      <c r="D121" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122">
+        <v>1</v>
+      </c>
+      <c r="C122">
+        <v>10</v>
+      </c>
+      <c r="D122" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123">
+        <v>1</v>
+      </c>
+      <c r="C123">
+        <v>10</v>
+      </c>
+      <c r="D123" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124">
+        <v>1</v>
+      </c>
+      <c r="C124">
+        <v>10</v>
+      </c>
+      <c r="D124" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125">
+        <v>1</v>
+      </c>
+      <c r="C125">
+        <v>10</v>
+      </c>
+      <c r="D125" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126">
+        <v>1</v>
+      </c>
+      <c r="C126">
+        <v>10</v>
+      </c>
+      <c r="D126" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127">
+        <v>1</v>
+      </c>
+      <c r="C127">
+        <v>10</v>
+      </c>
+      <c r="D127" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128">
+        <v>1</v>
+      </c>
+      <c r="C128">
+        <v>10</v>
+      </c>
+      <c r="D128" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129">
+        <v>1</v>
+      </c>
+      <c r="C129">
+        <v>10</v>
+      </c>
+      <c r="D129" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130">
+        <v>1</v>
+      </c>
+      <c r="C130">
+        <v>10</v>
+      </c>
+      <c r="D130" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131">
+        <v>1</v>
+      </c>
+      <c r="C131">
+        <v>10</v>
+      </c>
+      <c r="D131" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132">
+        <v>1</v>
+      </c>
+      <c r="C132">
+        <v>10</v>
+      </c>
+      <c r="D132" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133">
+        <v>1</v>
+      </c>
+      <c r="C133">
+        <v>10</v>
+      </c>
+      <c r="D133" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134">
+        <v>1</v>
+      </c>
+      <c r="C134">
+        <v>10</v>
+      </c>
+      <c r="D134" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135">
+        <v>1</v>
+      </c>
+      <c r="C135">
+        <v>10</v>
+      </c>
+      <c r="D135" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136">
+        <v>1</v>
+      </c>
+      <c r="C136">
+        <v>10</v>
+      </c>
+      <c r="D136" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137">
+        <v>1</v>
+      </c>
+      <c r="C137">
+        <v>10</v>
+      </c>
+      <c r="D137" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138">
+        <v>1</v>
+      </c>
+      <c r="C138">
+        <v>10</v>
+      </c>
+      <c r="D138" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139">
+        <v>1</v>
+      </c>
+      <c r="C139">
+        <v>10</v>
+      </c>
+      <c r="D139" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140">
+        <v>1</v>
+      </c>
+      <c r="C140">
+        <v>10</v>
+      </c>
+      <c r="D140" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141">
+        <v>1</v>
+      </c>
+      <c r="C141">
+        <v>10</v>
+      </c>
+      <c r="D141" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{142E83C8-DD36-4890-8C31-F3A23F457C50}">
   <dimension ref="A1:K17"/>
   <sheetViews>

</xml_diff>